<commit_message>
:large_blue_diamond: feat(app): Configuration de l'application
+ Configuration de l'environnement de travail .NET Maui
+ Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/matvelickov-journalTravail-p_app.xlsx
+++ b/matvelickov-journalTravail-p_app.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETML\CFC\23-24_secondYear\Projects\P_APP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETML\CFC\23-24_secondYear\Projects\P_APP\xamarin-eReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B99D73-247D-41D6-85C5-35BC857168CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADA1F62-6A4F-4257-8A4D-FADEDD93F540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="540" windowWidth="24120" windowHeight="11835" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -132,10 +132,76 @@
     <t>Velickovic Mateja</t>
   </si>
   <si>
-    <t>Développement de la maquette sur Figma</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">7.1.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Développement de la maquette sur Figma</t>
+    </r>
   </si>
   <si>
-    <t>Ajout des élements optionnels sur la maquette</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ajout des élements optionnels sur la maquette</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">7.1.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ajout d'une barre de recherche dans le menu d'accueil</t>
+    </r>
+  </si>
+  <si>
+    <t>Initialisation de l'environnement de développement .NET MAUI</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1097,7 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1046,7 +1112,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4722222222222224E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1962,7 +2028,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2015,7 +2081,7 @@
       </c>
       <c r="C3" s="24" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heures "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heures 20 minutes</v>
+        <v>0 jours 3 heures 50 minutes</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="3"/>
@@ -2030,15 +2096,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="24">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="24">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="E4" s="51">
         <f>SUM(C4:D4)</f>
-        <v>140</v>
+        <v>230</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2153,14 +2219,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="38"/>
+        <v>13</v>
+      </c>
+      <c r="B10" s="38">
+        <v>45376</v>
+      </c>
       <c r="C10" s="34"/>
-      <c r="D10" s="42"/>
-      <c r="F10" s="47"/>
+      <c r="D10" s="42">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="17"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -2173,15 +2248,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="str">
+      <c r="A11" s="8">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="35"/>
+        <v>13</v>
+      </c>
+      <c r="B11" s="39">
+        <v>45376</v>
+      </c>
+      <c r="C11" s="35">
+        <v>1</v>
+      </c>
       <c r="D11" s="43"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="47"/>
+      <c r="E11" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="19"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -8335,7 +8418,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8347,7 +8430,7 @@
       </c>
       <c r="D5" s="44">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8425,7 +8508,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C10" s="48" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8433,7 +8516,7 @@
       </c>
       <c r="D10" s="44">
         <f t="shared" si="0"/>
-        <v>3.4722222222222224E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8456,7 +8539,7 @@
       </c>
       <c r="D12" s="45">
         <f>SUM(D4:D11)</f>
-        <v>5.5555555555555552E-2</v>
+        <v>0.11805555555555555</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8735,15 +8818,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8753,6 +8827,15 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8776,14 +8859,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8795,4 +8870,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:large_orange_diamond: fix(journal): Mise à jour du journal de travail
+ Mise à jour du journal de travail
</commit_message>
<xml_diff>
--- a/matvelickov-journalTravail-p_app.xlsx
+++ b/matvelickov-journalTravail-p_app.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETML\CFC\23-24_secondYear\Projects\P_APP\xamarin-eReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADA1F62-6A4F-4257-8A4D-FADEDD93F540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D01420-405A-4933-A091-E6001BC0600B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -1097,7 +1097,7 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>7.6388888888888895E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2028,7 +2028,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="C3" s="24" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heures "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 3 heures 50 minutes</v>
+        <v>0 jours 4 heures 40 minutes</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="3"/>
@@ -2100,11 +2100,11 @@
       </c>
       <c r="D4" s="24">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="E4" s="51">
         <f>SUM(C4:D4)</f>
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2258,7 +2258,9 @@
       <c r="C11" s="35">
         <v>1</v>
       </c>
-      <c r="D11" s="43"/>
+      <c r="D11" s="43">
+        <v>50</v>
+      </c>
       <c r="E11" s="18" t="s">
         <v>4</v>
       </c>
@@ -8422,7 +8424,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="C5" s="52" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8430,7 +8432,7 @@
       </c>
       <c r="D5" s="44">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>4.1666666666666664E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8539,7 +8541,7 @@
       </c>
       <c r="D12" s="45">
         <f>SUM(D4:D11)</f>
-        <v>0.11805555555555555</v>
+        <v>0.15277777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
:large_blue_diamond: feat(app): Ajout de l'application .MAUI
+ Mise à jour du journal de travail.
+ Création de l'application .MAUI.
</commit_message>
<xml_diff>
--- a/matvelickov-journalTravail-p_app.xlsx
+++ b/matvelickov-journalTravail-p_app.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETML\CFC\23-24_secondYear\Projects\P_APP\xamarin-eReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D01420-405A-4933-A091-E6001BC0600B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E8EE9F-2E1F-4A31-A678-4A5A91F2126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="30165" yWindow="3510" windowWidth="24120" windowHeight="11835" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>Initialisation de l'environnement de développement .NET MAUI</t>
+  </si>
+  <si>
+    <t>Modification de l'icône de l'application ainsi que de son nom</t>
+  </si>
+  <si>
+    <t>Amélioration de quelques détails sur la maquette</t>
+  </si>
+  <si>
+    <t>Documentation sur le language de développement utilisé et développement de l'application</t>
   </si>
 </sst>
 </file>
@@ -385,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -491,11 +500,88 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -660,80 +746,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1097,7 +1109,7 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.6388888888888895E-2</c:v>
+                  <c:v>0.15972222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1112,7 +1124,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>6.9444444444444448E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1821,18 +1833,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h." dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h." dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2028,7 +2040,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2093,7 @@
       </c>
       <c r="C3" s="24" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heures "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 4 heures 40 minutes</v>
+        <v>0 jours 7 heures 0 minutes</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="3"/>
@@ -2096,15 +2108,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="24">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D4" s="24">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="E4" s="51">
         <f>SUM(C4:D4)</f>
-        <v>280</v>
+        <v>420</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2279,14 +2291,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="38"/>
+        <v>16</v>
+      </c>
+      <c r="B12" s="38">
+        <v>45397</v>
+      </c>
       <c r="C12" s="34"/>
-      <c r="D12" s="42"/>
-      <c r="F12" s="47"/>
+      <c r="D12" s="42">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="17"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2299,15 +2320,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="str">
+      <c r="A13" s="8">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="39"/>
+        <v>16</v>
+      </c>
+      <c r="B13" s="39">
+        <v>45397</v>
+      </c>
       <c r="C13" s="35"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="47"/>
+      <c r="D13" s="43">
+        <v>20</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>35</v>
+      </c>
       <c r="G13" s="19"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2320,14 +2349,25 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="42"/>
-      <c r="F14" s="47"/>
+        <v>16</v>
+      </c>
+      <c r="B14" s="38">
+        <v>45397</v>
+      </c>
+      <c r="C14" s="34">
+        <v>1</v>
+      </c>
+      <c r="D14" s="42">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="17"/>
       <c r="M14" t="s">
         <v>24</v>
@@ -8324,28 +8364,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8420,11 +8460,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C5" s="52" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8432,7 +8472,7 @@
       </c>
       <c r="D5" s="44">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>7.6388888888888895E-2</v>
+        <v>0.15972222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8510,7 +8550,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C10" s="48" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8518,7 +8558,7 @@
       </c>
       <c r="D10" s="44">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>6.9444444444444448E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8541,7 +8581,7 @@
       </c>
       <c r="D12" s="45">
         <f>SUM(D4:D11)</f>
-        <v>0.15277777777777779</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8820,6 +8860,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8829,15 +8878,6 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8861,6 +8901,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8872,12 +8920,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
:large_blue_diamond: feat(app): Développement de l'application
+ Ajout d'une barre de recherche dans le menu d'accueil.
+ Ajout d'une gallerie de livres en dessous de la barre de recherche.
+ Ajout de la police d'écriture Poppins à l'application.
</commit_message>
<xml_diff>
--- a/matvelickov-journalTravail-p_app.xlsx
+++ b/matvelickov-journalTravail-p_app.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ETML\CFC\23-24_secondYear\Projects\P_APP\xamarin-eReader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E8EE9F-2E1F-4A31-A678-4A5A91F2126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B65F9C-ED23-4D81-B0AE-B90A86B983B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30165" yWindow="3510" windowWidth="24120" windowHeight="11835" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>Documentation sur le language de développement utilisé et développement de l'application</t>
+  </si>
+  <si>
+    <t>Développement de l'application afin de la faire ressembler à la maquette.</t>
+  </si>
+  <si>
+    <t>Ajout de la police d'écriture Poppins à l'application.</t>
+  </si>
+  <si>
+    <t>Ajout d'une gallerie d'image sur la page d'accueil.</t>
   </si>
 </sst>
 </file>
@@ -493,6 +502,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -500,88 +512,11 @@
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -746,6 +681,80 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1109,13 +1118,13 @@
                   <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15972222222222221</c:v>
+                  <c:v>0.19444444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1833,18 +1842,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h." dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h." dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2039,8 +2048,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2075,11 +2084,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2093,7 +2102,7 @@
       </c>
       <c r="C3" s="24" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heures "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heures 0 minutes</v>
+        <v>0 jours 9 heures 20 minutes</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="3"/>
@@ -2108,24 +2117,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="24">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="D4" s="24">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="E4" s="51">
         <f>SUM(C4:D4)</f>
-        <v>420</v>
+        <v>560</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="55"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" spans="1:15" s="22" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
@@ -2363,9 +2372,9 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="54" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="17"/>
@@ -2380,15 +2389,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="str">
+      <c r="A15" s="8">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="B15" s="39">
+        <v>45404</v>
+      </c>
+      <c r="C15" s="35">
+        <v>1</v>
+      </c>
+      <c r="D15" s="43">
+        <v>30</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="19"/>
       <c r="M15" t="s">
         <v>25</v>
@@ -2401,29 +2420,46 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="38"/>
+        <v>17</v>
+      </c>
+      <c r="B16" s="38">
+        <v>45404</v>
+      </c>
       <c r="C16" s="34"/>
-      <c r="D16" s="42"/>
-      <c r="F16" s="47"/>
+      <c r="D16" s="42">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="17"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="str">
+      <c r="A17" s="8">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="39"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="39">
+        <v>45404</v>
+      </c>
       <c r="C17" s="35"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="47"/>
+      <c r="D17" s="43">
+        <v>30</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="19"/>
       <c r="O17">
         <v>45</v>
@@ -8364,28 +8400,28 @@
     <mergeCell ref="C5:D5"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8464,7 +8500,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="C5" s="52" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8472,7 +8508,7 @@
       </c>
       <c r="D5" s="44">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.15972222222222221</v>
+        <v>0.19444444444444445</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8496,11 +8532,11 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C7" s="29" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8508,7 +8544,7 @@
       </c>
       <c r="D7" s="44">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8581,7 +8617,7 @@
       </c>
       <c r="D12" s="45">
         <f>SUM(D4:D11)</f>
-        <v>0.25</v>
+        <v>0.34722222222222221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8860,15 +8896,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8878,6 +8905,15 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8901,14 +8937,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8920,4 +8948,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>